<commit_message>
Pubmed ids, sdrf performers and study designs now can be added.  Fixed addition filter.
git-svn-id: https://cbilsvn.pmacs.upenn.edu/svn/gus/GusAppFramework/branches/4.0@13041 4235af6a-31f9-0310-9ad3-ecf6348f2534
</commit_message>
<xml_diff>
--- a/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx1.xlsx
+++ b/Community/MagetabConverter/Magetab2Xml/samples/test_magetab_appdx1.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-7635" yWindow="2415" windowWidth="19440" windowHeight="8085" tabRatio="162" activeTab="1"/>
+    <workbookView xWindow="-7635" yWindow="2415" windowWidth="19440" windowHeight="8085" tabRatio="162"/>
   </bookViews>
   <sheets>
     <sheet name="IDF" sheetId="1" r:id="rId1"/>
@@ -344,9 +344,6 @@
     <t>VANTAGE: Vanderbilt Technologies for Advanced Genomics</t>
   </si>
   <si>
-    <t>Whole transcriptome analysis of Sox17-expressing cells in E8.0 and E8.5 mouse embryos</t>
-  </si>
-  <si>
     <t>This experiment has been done to understand the dynamics of gene expression in Sox17-expressing cells using multiplex RNA-Seq technology. Sox17.GFP(+) cells were isolated by FACS from E8.0 and E8.5 mouse embryos. The temporal comparison between E8.0 and E8.5 provides insight into which genes are differentially of specifically expressed during endoderm patterning.</t>
   </si>
   <si>
@@ -900,12 +897,15 @@
   </si>
   <si>
     <t>1;1;1;1</t>
+  </si>
+  <si>
+    <t>Whole transcriptome analysis of Sox17-expressing cells in E8.0 and E8.5 mouse embryos &lt;id=studyId&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="41">
     <font>
       <sz val="11"/>
@@ -1890,7 +1890,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1925,7 +1924,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2101,11 +2099,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IV61"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2126,7 +2124,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B1" s="8">
         <v>1.1000000000000001</v>
@@ -2137,47 +2135,47 @@
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="60">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -2189,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
@@ -2202,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C10" s="15"/>
       <c r="D10" s="15"/>
@@ -2232,10 +2230,10 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C13" s="18"/>
       <c r="D13" s="18"/>
@@ -2252,7 +2250,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F15" s="11"/>
     </row>
@@ -2267,18 +2265,18 @@
         <v>25</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="17" spans="1:256">
       <c r="A17" s="10" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>108</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" spans="1:256">
@@ -2292,7 +2290,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F18" s="67"/>
     </row>
@@ -2304,16 +2302,16 @@
         <v>52</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F19" s="67"/>
     </row>
     <row r="20" spans="1:256">
       <c r="A20" s="23" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F20" s="67"/>
     </row>
@@ -2322,46 +2320,46 @@
         <v>9</v>
       </c>
       <c r="B21" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>132</v>
-      </c>
       <c r="D21" s="8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F21" s="67"/>
     </row>
     <row r="22" spans="1:256">
       <c r="A22" s="24" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="8" t="s">
-        <v>126</v>
-      </c>
       <c r="C22" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F22" s="67"/>
     </row>
     <row r="23" spans="1:256">
       <c r="A23" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B23" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D23" s="25" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F23" s="68"/>
       <c r="G23" s="24"/>
@@ -2617,19 +2615,19 @@
     </row>
     <row r="24" spans="1:256">
       <c r="A24" s="26" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F24" s="69"/>
       <c r="G24" s="26"/>
@@ -2885,19 +2883,19 @@
     </row>
     <row r="25" spans="1:256">
       <c r="A25" s="26" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="69"/>
       <c r="G25" s="26"/>
@@ -3153,16 +3151,16 @@
     </row>
     <row r="26" spans="1:256">
       <c r="A26" s="26" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="69"/>
@@ -3428,7 +3426,7 @@
         <v>27</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>27</v>
@@ -3448,33 +3446,33 @@
         <v>41</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F28" s="60" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="29" spans="1:256">
       <c r="A29" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>112</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>113</v>
-      </c>
       <c r="C29" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D29" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F29" s="60" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:256">
@@ -3485,7 +3483,7 @@
     </row>
     <row r="31" spans="1:256">
       <c r="A31" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B31" s="28"/>
       <c r="C31" s="14"/>
@@ -3493,7 +3491,7 @@
     </row>
     <row r="32" spans="1:256">
       <c r="A32" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="14"/>
@@ -3507,7 +3505,7 @@
     </row>
     <row r="34" spans="1:41">
       <c r="A34" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="28">
         <v>14983035</v>
@@ -3517,7 +3515,7 @@
     </row>
     <row r="35" spans="1:41">
       <c r="A35" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B35" s="28"/>
       <c r="C35" s="14"/>
@@ -3525,7 +3523,7 @@
     </row>
     <row r="36" spans="1:41">
       <c r="A36" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B36" s="28"/>
       <c r="C36" s="14"/>
@@ -3533,7 +3531,7 @@
     </row>
     <row r="37" spans="1:41">
       <c r="A37" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B37" s="28"/>
       <c r="C37" s="14"/>
@@ -3549,19 +3547,19 @@
         <v>13</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>70</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F39" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G39" s="33" t="s">
         <v>53</v>
@@ -3570,13 +3568,13 @@
         <v>54</v>
       </c>
       <c r="I39" s="64" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J39" s="64" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K39" s="64" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="L39" s="35"/>
       <c r="M39" s="35"/>
@@ -3614,34 +3612,34 @@
         <v>14</v>
       </c>
       <c r="B40" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C40" s="14" t="s">
+        <v>162</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>163</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>164</v>
-      </c>
       <c r="E40" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F40" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="G40" s="36" t="s">
+        <v>179</v>
+      </c>
+      <c r="H40" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="I40" s="65" t="s">
+        <v>158</v>
+      </c>
+      <c r="J40" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="G40" s="36" t="s">
+      <c r="K40" s="64" t="s">
         <v>180</v>
-      </c>
-      <c r="H40" s="37" t="s">
-        <v>181</v>
-      </c>
-      <c r="I40" s="65" t="s">
-        <v>159</v>
-      </c>
-      <c r="J40" s="70" t="s">
-        <v>175</v>
-      </c>
-      <c r="K40" s="64" t="s">
-        <v>181</v>
       </c>
       <c r="L40" s="35"/>
       <c r="M40" s="35"/>
@@ -3679,34 +3677,34 @@
         <v>17</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H41" s="9" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I41" s="66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J41" s="66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K41" s="66" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
@@ -3717,29 +3715,29 @@
         <v>62</v>
       </c>
       <c r="C42" s="39" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D42" s="39"/>
       <c r="E42" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="F42" s="31" t="s">
-        <v>177</v>
-      </c>
-      <c r="G42" s="36" t="s">
+      <c r="H42" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="H42" s="37" t="s">
-        <v>192</v>
-      </c>
       <c r="I42" s="64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J42" s="64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="K42" s="64" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="L42" s="35"/>
       <c r="M42" s="35"/>
@@ -3774,23 +3772,23 @@
     </row>
     <row r="43" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A43" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C43" s="41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D43" s="39"/>
       <c r="E43" s="40"/>
       <c r="F43" s="31"/>
       <c r="G43" s="36"/>
       <c r="H43" s="37" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I43" s="64" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="35"/>
@@ -3827,7 +3825,7 @@
     </row>
     <row r="44" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A44" s="42" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B44" s="38"/>
       <c r="C44" s="39"/>
@@ -3872,7 +3870,7 @@
     </row>
     <row r="45" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A45" s="26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B45" s="38">
         <v>1</v>
@@ -3896,13 +3894,13 @@
         <v>0</v>
       </c>
       <c r="I45" s="64" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J45" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="K45" s="64" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="L45" s="35"/>
       <c r="M45" s="35"/>
@@ -3937,7 +3935,7 @@
     </row>
     <row r="46" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A46" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B46" s="38"/>
       <c r="C46" s="39"/>
@@ -3982,7 +3980,7 @@
     </row>
     <row r="47" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A47" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B47" s="38"/>
       <c r="C47" s="39"/>
@@ -4027,13 +4025,13 @@
     </row>
     <row r="48" spans="1:41" s="3" customFormat="1" ht="59.25" customHeight="1">
       <c r="A48" s="26" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C48" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D48" s="39"/>
       <c r="E48" s="40"/>
@@ -4079,17 +4077,17 @@
         <v>16</v>
       </c>
       <c r="B49" s="39" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C49" s="43"/>
       <c r="D49" s="30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E49" s="35" t="s">
         <v>105</v>
       </c>
       <c r="F49" s="44" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G49" s="45" t="s">
         <v>60</v>
@@ -4098,13 +4096,13 @@
         <v>61</v>
       </c>
       <c r="I49" s="64" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J49" s="64" t="s">
+        <v>287</v>
+      </c>
+      <c r="K49" s="64" t="s">
         <v>288</v>
-      </c>
-      <c r="K49" s="64" t="s">
-        <v>289</v>
       </c>
       <c r="L49" s="35"/>
       <c r="M49" s="35"/>
@@ -4139,33 +4137,33 @@
     </row>
     <row r="50" spans="1:41">
       <c r="A50" s="26" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="51" spans="1:41">
       <c r="A51" s="26" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:41">
       <c r="A52" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="53" spans="1:41">
       <c r="A53" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:41">
       <c r="A54" s="26" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B54" s="8">
         <v>0</v>
@@ -4174,30 +4172,30 @@
         <v>1</v>
       </c>
       <c r="E54" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="F54" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="G54" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="G54" s="8" t="s">
+      <c r="H54" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="H54" s="8" t="s">
-        <v>188</v>
-      </c>
       <c r="I54" s="67" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J54" s="66" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K54" s="66" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="55" spans="1:41">
       <c r="A55" s="26" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:41">
@@ -4205,7 +4203,7 @@
     </row>
     <row r="57" spans="1:41">
       <c r="A57" s="23" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="58" spans="1:41">
@@ -4216,13 +4214,13 @@
         <v>18</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:41">
@@ -4230,10 +4228,10 @@
         <v>19</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="61" spans="1:41">
@@ -4244,10 +4242,10 @@
         <v>2.31</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -4266,10 +4264,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:ED8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="X11" sqref="X11"/>
     </sheetView>
   </sheetViews>
@@ -4323,19 +4321,19 @@
         <v>28</v>
       </c>
       <c r="B1" s="46" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D1" s="46" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E1" s="46" t="s">
         <v>29</v>
       </c>
       <c r="F1" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G1" s="46" t="s">
         <v>30</v>
@@ -4344,13 +4342,13 @@
         <v>31</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J1" s="46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="K1" s="46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="46" t="s">
         <v>32</v>
@@ -4359,7 +4357,7 @@
         <v>107</v>
       </c>
       <c r="N1" s="47" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O1" s="48" t="s">
         <v>33</v>
@@ -4368,13 +4366,13 @@
         <v>29</v>
       </c>
       <c r="Q1" s="48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R1" s="48" t="s">
         <v>45</v>
       </c>
       <c r="S1" s="48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="T1" s="48" t="s">
         <v>32</v>
@@ -4389,13 +4387,13 @@
         <v>29</v>
       </c>
       <c r="X1" s="48" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Y1" s="48" t="s">
         <v>32</v>
       </c>
       <c r="Z1" s="48" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="AA1" s="48" t="s">
         <v>32</v>
@@ -4455,10 +4453,10 @@
         <v>97</v>
       </c>
       <c r="AT1" s="47" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AU1" s="46" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="AV1" s="46" t="s">
         <v>32</v>
@@ -4479,13 +4477,13 @@
         <v>35</v>
       </c>
       <c r="BB1" s="71" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="BC1" s="51" t="s">
         <v>42</v>
       </c>
       <c r="BD1" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BE1" s="52" t="s">
         <v>32</v>
@@ -4506,93 +4504,93 @@
         <v>42</v>
       </c>
       <c r="BK1" s="51" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="BL1" s="51" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="BM1" s="48" t="s">
         <v>106</v>
       </c>
       <c r="BN1" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="BO1" s="46" t="s">
         <v>263</v>
-      </c>
-      <c r="BO1" s="46" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:134" ht="15.75">
       <c r="A2" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J2" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K2" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K2" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L2" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M2" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N2" s="30">
         <v>0.98950000000000005</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>39</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T2" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U2" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y2" s="31" t="s">
         <v>70</v>
@@ -4601,7 +4599,7 @@
         <v>7</v>
       </c>
       <c r="AA2" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB2" s="30">
         <v>155</v>
@@ -4623,10 +4621,10 @@
       </c>
       <c r="AH2" s="48"/>
       <c r="AI2" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="AJ2" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK2" s="19" t="s">
         <v>108</v>
@@ -4656,16 +4654,16 @@
         <v>33</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AV2" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AW2" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX2" s="4" t="s">
         <v>57</v>
@@ -4680,16 +4678,16 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="BC2" s="30" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="BE2" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF2" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG2" s="4">
         <v>1.0900000000000001</v>
@@ -4701,96 +4699,96 @@
         <v>75</v>
       </c>
       <c r="BJ2" s="30" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="BL2" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN2" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM2" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN2" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO2" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="3" spans="1:134" ht="15.75">
       <c r="A3" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C3" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J3" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K3" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K3" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L3" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M3" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N3" s="30" t="s">
         <v>66</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R3" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T3" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U3" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="W3" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X3" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y3" s="31" t="s">
         <v>70</v>
@@ -4799,7 +4797,7 @@
         <v>10</v>
       </c>
       <c r="AA3" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB3" s="30">
         <v>155</v>
@@ -4821,10 +4819,10 @@
       </c>
       <c r="AH3" s="48"/>
       <c r="AI3" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="AJ3" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK3" s="19" t="s">
         <v>108</v>
@@ -4854,16 +4852,16 @@
         <v>33</v>
       </c>
       <c r="AT3" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AU3" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AV3" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AW3" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX3" s="4" t="s">
         <v>57</v>
@@ -4878,16 +4876,16 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="BC3" s="30" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="BD3" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="BE3" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF3" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG3" s="4">
         <v>1.0900000000000001</v>
@@ -4899,96 +4897,96 @@
         <v>75</v>
       </c>
       <c r="BJ3" s="30" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="BK3" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="BL3" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM3" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN3" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM3" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN3" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO3" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:134" ht="15.75">
       <c r="A4" s="30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B4" s="30" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J4" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K4" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K4" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L4" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M4" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N4" s="30">
         <v>0.96220000000000006</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="P4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T4" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U4" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X4" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y4" s="31" t="s">
         <v>70</v>
@@ -4997,7 +4995,7 @@
         <v>10</v>
       </c>
       <c r="AA4" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB4" s="30">
         <v>155</v>
@@ -5019,10 +5017,10 @@
       </c>
       <c r="AH4" s="48"/>
       <c r="AI4" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AJ4" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK4" s="19" t="s">
         <v>108</v>
@@ -5052,16 +5050,16 @@
         <v>33</v>
       </c>
       <c r="AT4" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AU4" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AV4" s="33" t="s">
         <v>53</v>
       </c>
       <c r="AW4" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX4" s="4" t="s">
         <v>57</v>
@@ -5076,16 +5074,16 @@
         <v>1.0900000000000001</v>
       </c>
       <c r="BC4" s="30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="BD4" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="BE4" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF4" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG4" s="4">
         <v>1.0900000000000001</v>
@@ -5097,63 +5095,63 @@
         <v>75</v>
       </c>
       <c r="BJ4" s="30" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="BK4" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="BL4" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM4" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN4" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM4" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN4" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO4" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:134" ht="15.75">
       <c r="A5" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>63</v>
       </c>
       <c r="C5" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="D5" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="D5" s="30" t="s">
-        <v>257</v>
-      </c>
       <c r="E5" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J5" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K5" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K5" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L5" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M5" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N5" s="30">
         <v>0.97909999999999997</v>
@@ -5165,28 +5163,28 @@
         <v>39</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T5" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U5" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>80</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y5" s="31" t="s">
         <v>70</v>
@@ -5195,7 +5193,7 @@
         <v>10</v>
       </c>
       <c r="AA5" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB5" s="30">
         <v>155</v>
@@ -5222,7 +5220,7 @@
         <v>85</v>
       </c>
       <c r="AJ5" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK5" s="19" t="s">
         <v>108</v>
@@ -5252,7 +5250,7 @@
         <v>33</v>
       </c>
       <c r="AT5" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="AU5" s="4" t="s">
         <v>102</v>
@@ -5261,7 +5259,7 @@
         <v>53</v>
       </c>
       <c r="AW5" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX5" s="4" t="s">
         <v>57</v>
@@ -5279,13 +5277,13 @@
         <v>72</v>
       </c>
       <c r="BD5" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="BE5" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF5" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG5" s="4">
         <v>1.0900000000000001</v>
@@ -5300,60 +5298,60 @@
         <v>76</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="BL5" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM5" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN5" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM5" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN5" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO5" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:134" ht="15.75">
       <c r="A6" s="30" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>64</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J6" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K6" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K6" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L6" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N6" s="30" t="s">
         <v>66</v>
@@ -5365,28 +5363,28 @@
         <v>39</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T6" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U6" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V6" s="4" t="s">
         <v>81</v>
       </c>
       <c r="W6" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X6" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y6" s="31" t="s">
         <v>70</v>
@@ -5395,7 +5393,7 @@
         <v>10</v>
       </c>
       <c r="AA6" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB6" s="30">
         <v>155</v>
@@ -5422,7 +5420,7 @@
         <v>84</v>
       </c>
       <c r="AJ6" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK6" s="19" t="s">
         <v>108</v>
@@ -5452,7 +5450,7 @@
         <v>33</v>
       </c>
       <c r="AT6" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AU6" s="4" t="s">
         <v>103</v>
@@ -5461,7 +5459,7 @@
         <v>53</v>
       </c>
       <c r="AW6" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX6" s="4" t="s">
         <v>57</v>
@@ -5479,13 +5477,13 @@
         <v>73</v>
       </c>
       <c r="BD6" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="BE6" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF6" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG6" s="4">
         <v>1.0900000000000001</v>
@@ -5500,60 +5498,60 @@
         <v>77</v>
       </c>
       <c r="BK6" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="BL6" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM6" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN6" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM6" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN6" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO6" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="7" spans="1:134" ht="15.75">
       <c r="A7" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" s="30" t="s">
         <v>65</v>
       </c>
       <c r="C7" s="30" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J7" s="53" t="s">
+        <v>223</v>
+      </c>
+      <c r="K7" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="K7" s="30" t="s">
-        <v>225</v>
-      </c>
       <c r="L7" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M7" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="N7" s="30">
         <v>0.99319999999999997</v>
@@ -5565,25 +5563,25 @@
         <v>39</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T7" s="19" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>82</v>
       </c>
       <c r="W7" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X7" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y7" s="31" t="s">
         <v>70</v>
@@ -5592,7 +5590,7 @@
         <v>10</v>
       </c>
       <c r="AA7" s="31" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AB7" s="30">
         <v>155</v>
@@ -5619,7 +5617,7 @@
         <v>83</v>
       </c>
       <c r="AJ7" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK7" s="19" t="s">
         <v>108</v>
@@ -5649,7 +5647,7 @@
         <v>33</v>
       </c>
       <c r="AT7" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="AU7" s="4" t="s">
         <v>104</v>
@@ -5658,7 +5656,7 @@
         <v>53</v>
       </c>
       <c r="AW7" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AX7" s="4" t="s">
         <v>57</v>
@@ -5676,13 +5674,13 @@
         <v>74</v>
       </c>
       <c r="BD7" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="BE7" s="30" t="s">
         <v>54</v>
       </c>
       <c r="BF7" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG7" s="4">
         <v>1.0900000000000001</v>
@@ -5697,89 +5695,89 @@
         <v>78</v>
       </c>
       <c r="BK7" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="BL7" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM7" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN7" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="BM7" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN7" s="4" t="s">
-        <v>262</v>
-      </c>
       <c r="BO7" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="8" spans="1:134" s="63" customFormat="1" ht="15.75">
       <c r="A8" s="56" t="s">
+        <v>270</v>
+      </c>
+      <c r="B8" s="56" t="s">
         <v>271</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>272</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="56"/>
       <c r="E8" s="56" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G8" s="56" t="s">
         <v>38</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J8" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="K8" s="56" t="s">
         <v>224</v>
       </c>
-      <c r="K8" s="56" t="s">
-        <v>225</v>
-      </c>
       <c r="L8" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="M8" s="56" t="s">
         <v>273</v>
       </c>
-      <c r="M8" s="56" t="s">
+      <c r="N8" s="56" t="s">
         <v>274</v>
       </c>
-      <c r="N8" s="56" t="s">
+      <c r="O8" s="56" t="s">
         <v>275</v>
-      </c>
-      <c r="O8" s="56" t="s">
-        <v>276</v>
       </c>
       <c r="P8" s="56" t="s">
         <v>39</v>
       </c>
       <c r="Q8" s="56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R8" s="56" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="S8" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="T8" s="58" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U8" s="56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="V8" s="56" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="W8" s="56" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="X8" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y8" s="59" t="s">
         <v>70</v>
@@ -5788,7 +5786,7 @@
         <v>10</v>
       </c>
       <c r="AA8" s="59" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="AC8" s="56"/>
       <c r="AD8" s="56"/>
@@ -5805,10 +5803,10 @@
         <v>101</v>
       </c>
       <c r="AI8" s="56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="AJ8" s="60" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK8" s="58" t="s">
         <v>108</v>
@@ -5838,57 +5836,57 @@
         <v>33</v>
       </c>
       <c r="AT8" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="AU8" s="56" t="s">
+        <v>289</v>
+      </c>
+      <c r="AV8" s="61" t="s">
         <v>280</v>
       </c>
-      <c r="AU8" s="56" t="s">
-        <v>290</v>
-      </c>
-      <c r="AV8" s="61" t="s">
-        <v>281</v>
-      </c>
       <c r="AW8" s="61" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="AZ8" s="56"/>
       <c r="BA8" s="62"/>
       <c r="BB8" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="BC8" s="56" t="s">
+        <v>290</v>
+      </c>
+      <c r="BD8" s="56" t="s">
         <v>282</v>
-      </c>
-      <c r="BC8" s="56" t="s">
-        <v>291</v>
-      </c>
-      <c r="BD8" s="56" t="s">
-        <v>283</v>
       </c>
       <c r="BE8" s="56" t="s">
         <v>54</v>
       </c>
       <c r="BF8" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="BG8" s="56">
         <v>1.0900000000000001</v>
       </c>
       <c r="BH8" s="56" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="BI8" s="56" t="s">
         <v>75</v>
       </c>
       <c r="BJ8" s="56" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="BK8" s="56" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="BL8" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="BM8" s="56" t="s">
+        <v>266</v>
+      </c>
+      <c r="BN8" s="56" t="s">
         <v>261</v>
-      </c>
-      <c r="BM8" s="56" t="s">
-        <v>267</v>
-      </c>
-      <c r="BN8" s="56" t="s">
-        <v>262</v>
       </c>
       <c r="BO8" s="63">
         <v>2</v>

</xml_diff>